<commit_message>
Updated samplelist. Added code to generate/plot figures and added SigProfiler commands.
</commit_message>
<xml_diff>
--- a/Conversion_ManuscriptID_EGA-ID/NCOMMS-23-52197_Conversion_ManuscriptID_EGA-ID.xlsx
+++ b/Conversion_ManuscriptID_EGA-ID/NCOMMS-23-52197_Conversion_ManuscriptID_EGA-ID.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dilysweijers/surfdrive/Paper_CMMRD/Dilys_05_07_2024/Submission files/Additional on request editor/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dilysweijers/surfdrive/Paper_CMMRD/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9DC612E6-67B9-E54E-AEBE-43A2642142A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6FC3822A-8E4B-1F47-9AAA-9630AEA7AC84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15640" xr2:uid="{101B49D3-1B7A-9C48-97FC-6A6B0565C845}"/>
+    <workbookView xWindow="780" yWindow="940" windowWidth="23740" windowHeight="15640" xr2:uid="{101B49D3-1B7A-9C48-97FC-6A6B0565C845}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="153">
   <si>
     <t>Individual ID</t>
   </si>
@@ -396,6 +396,105 @@
   </si>
   <si>
     <t>EGAD50000000113</t>
+  </si>
+  <si>
+    <t>GI1</t>
+  </si>
+  <si>
+    <t>GI2</t>
+  </si>
+  <si>
+    <t>Brain1</t>
+  </si>
+  <si>
+    <t>File ID</t>
+  </si>
+  <si>
+    <t>T_CMMRD1_CA16_WXS.cram.gpg</t>
+  </si>
+  <si>
+    <t>T_CMMRD1_CRC18_WXS.cram.gpg</t>
+  </si>
+  <si>
+    <t>T_CMMRD1_GBM19_WXS.cram.gpg</t>
+  </si>
+  <si>
+    <t>GI3</t>
+  </si>
+  <si>
+    <t>T_CMMRD8_CA14_WXS.cram.gpg</t>
+  </si>
+  <si>
+    <t>GI4</t>
+  </si>
+  <si>
+    <t>GI5</t>
+  </si>
+  <si>
+    <t>T_CMMRD9_CRC22_WXS.cram.gpg</t>
+  </si>
+  <si>
+    <t>T_CMMRD9_SC23_WXS.cram.gpg</t>
+  </si>
+  <si>
+    <t>GI6</t>
+  </si>
+  <si>
+    <t>GI7</t>
+  </si>
+  <si>
+    <t>T_CMMRD10_CRC29_WXS.cram.gpg</t>
+  </si>
+  <si>
+    <t>T_CMMRD10_LK29_WXS.cram.gpg</t>
+  </si>
+  <si>
+    <t>Brain2</t>
+  </si>
+  <si>
+    <t>T_CMMRD11_GBM8_WXS.cram.gpg</t>
+  </si>
+  <si>
+    <t>CRC1</t>
+  </si>
+  <si>
+    <t>CRC2</t>
+  </si>
+  <si>
+    <t>CRC3</t>
+  </si>
+  <si>
+    <t>CRC4</t>
+  </si>
+  <si>
+    <t>CRC5</t>
+  </si>
+  <si>
+    <t>CRC6</t>
+  </si>
+  <si>
+    <t>CRC7</t>
+  </si>
+  <si>
+    <t>CMMRDT19_50966IAI_WXS.cram.gpg</t>
+  </si>
+  <si>
+    <t>CMMRDT19_50966IAL_WXS.cram.gpg</t>
+  </si>
+  <si>
+    <t>CMMRDT19_50966IAX_WXS.cram.gpg</t>
+  </si>
+  <si>
+    <t>CMMRDT19_50966IAZ_WXS.cram.gpg</t>
+  </si>
+  <si>
+    <t>CMMRDT19_50966IBN_WXS.cram.gpg</t>
+  </si>
+  <si>
+    <t>CMMRDT19_50966IR_WXS.cram.gpg</t>
+  </si>
+  <si>
+    <t>CMMRDT19_50966IV_WXS.cram.gpg</t>
   </si>
 </sst>
 </file>
@@ -468,15 +567,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -816,7 +914,7 @@
   <dimension ref="A1:L58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -824,16 +922,17 @@
     <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="16.83203125" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="38" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.1640625" style="4" customWidth="1"/>
-    <col min="10" max="10" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.83203125" style="4" customWidth="1"/>
-    <col min="12" max="12" width="30.5" style="4" customWidth="1"/>
+    <col min="4" max="4" width="31.6640625" customWidth="1"/>
+    <col min="5" max="5" width="16.83203125" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="38" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.1640625" customWidth="1"/>
+    <col min="11" max="11" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.83203125" customWidth="1"/>
+    <col min="13" max="13" width="30.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -844,17 +943,20 @@
         <v>80</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="7"/>
-    </row>
-    <row r="2" spans="1:11" ht="20" x14ac:dyDescent="0.25">
+      <c r="L1" s="6"/>
+    </row>
+    <row r="2" spans="1:12" ht="20" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -862,18 +964,19 @@
       <c r="C2" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>117</v>
-      </c>
+      <c r="D2" s="2"/>
       <c r="E2" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="5"/>
-    </row>
-    <row r="3" spans="1:11" ht="20" x14ac:dyDescent="0.25">
+      <c r="K2" s="4"/>
+    </row>
+    <row r="3" spans="1:12" ht="20" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -883,72 +986,88 @@
       <c r="C3" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>117</v>
-      </c>
+      <c r="D3" s="2"/>
       <c r="E3" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="5"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K3" s="4"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="2"/>
+      <c r="C4" s="2" t="s">
+        <v>120</v>
+      </c>
       <c r="D4" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="2"/>
+      <c r="C5" s="2" t="s">
+        <v>121</v>
+      </c>
       <c r="D5" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="G5" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="2"/>
+      <c r="C6" s="2" t="s">
+        <v>122</v>
+      </c>
       <c r="D6" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="F6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="G6" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="20" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>16</v>
       </c>
@@ -956,20 +1075,21 @@
       <c r="C7" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>117</v>
-      </c>
+      <c r="D7" s="2"/>
       <c r="E7" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="G7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I7" s="3"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="3"/>
-    </row>
-    <row r="8" spans="1:11" ht="20" x14ac:dyDescent="0.25">
+      <c r="J7" s="3"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="3"/>
+    </row>
+    <row r="8" spans="1:12" ht="20" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>16</v>
       </c>
@@ -979,20 +1099,21 @@
       <c r="C8" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>117</v>
-      </c>
+      <c r="D8" s="2"/>
       <c r="E8" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="G8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I8" s="3"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="3"/>
-    </row>
-    <row r="9" spans="1:11" ht="20" x14ac:dyDescent="0.25">
+      <c r="J8" s="3"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="3"/>
+    </row>
+    <row r="9" spans="1:12" ht="20" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
@@ -1002,20 +1123,21 @@
       <c r="C9" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="2"/>
+      <c r="E9" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="F9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="G9" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I9" s="3"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="3"/>
-    </row>
-    <row r="10" spans="1:11" ht="20" x14ac:dyDescent="0.25">
+      <c r="J9" s="3"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="3"/>
+    </row>
+    <row r="10" spans="1:12" ht="20" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>16</v>
       </c>
@@ -1025,18 +1147,19 @@
       <c r="C10" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>117</v>
-      </c>
+      <c r="D10" s="2"/>
       <c r="E10" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="G10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J10" s="5"/>
-    </row>
-    <row r="11" spans="1:11" ht="20" x14ac:dyDescent="0.25">
+      <c r="K10" s="4"/>
+    </row>
+    <row r="11" spans="1:12" ht="20" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
@@ -1046,18 +1169,19 @@
       <c r="C11" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>117</v>
-      </c>
+      <c r="D11" s="2"/>
       <c r="E11" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="G11" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="J11" s="5"/>
-    </row>
-    <row r="12" spans="1:11" ht="20" x14ac:dyDescent="0.25">
+      <c r="K11" s="4"/>
+    </row>
+    <row r="12" spans="1:12" ht="20" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>23</v>
       </c>
@@ -1065,18 +1189,19 @@
       <c r="C12" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>117</v>
-      </c>
+      <c r="D12" s="2"/>
       <c r="E12" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="G12" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J12" s="5"/>
-    </row>
-    <row r="13" spans="1:11" ht="20" x14ac:dyDescent="0.25">
+      <c r="K12" s="4"/>
+    </row>
+    <row r="13" spans="1:12" ht="20" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>23</v>
       </c>
@@ -1086,18 +1211,19 @@
       <c r="C13" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>117</v>
-      </c>
+      <c r="D13" s="2"/>
       <c r="E13" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="G13" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="J13" s="5"/>
-    </row>
-    <row r="14" spans="1:11" ht="20" x14ac:dyDescent="0.25">
+      <c r="K13" s="4"/>
+    </row>
+    <row r="14" spans="1:12" ht="20" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>26</v>
       </c>
@@ -1107,20 +1233,21 @@
       <c r="C14" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>117</v>
-      </c>
+      <c r="D14" s="2"/>
       <c r="E14" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="F14" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="G14" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="I14" s="3"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="3"/>
-    </row>
-    <row r="15" spans="1:11" ht="20" x14ac:dyDescent="0.25">
+      <c r="J14" s="3"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="3"/>
+    </row>
+    <row r="15" spans="1:12" ht="20" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>26</v>
       </c>
@@ -1130,18 +1257,19 @@
       <c r="C15" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>117</v>
-      </c>
+      <c r="D15" s="2"/>
       <c r="E15" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="F15" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="G15" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="J15" s="5"/>
-    </row>
-    <row r="16" spans="1:11" ht="20" x14ac:dyDescent="0.25">
+      <c r="K15" s="4"/>
+    </row>
+    <row r="16" spans="1:12" ht="20" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>26</v>
       </c>
@@ -1151,18 +1279,19 @@
       <c r="C16" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="2"/>
+      <c r="E16" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="F16" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="G16" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="J16" s="5"/>
-    </row>
-    <row r="17" spans="1:11" ht="20" x14ac:dyDescent="0.25">
+      <c r="K16" s="4"/>
+    </row>
+    <row r="17" spans="1:12" ht="20" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>32</v>
       </c>
@@ -1170,18 +1299,19 @@
       <c r="C17" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>117</v>
-      </c>
+      <c r="D17" s="2"/>
       <c r="E17" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="F17" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="G17" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J17" s="5"/>
-    </row>
-    <row r="18" spans="1:11" ht="20" x14ac:dyDescent="0.25">
+      <c r="K17" s="4"/>
+    </row>
+    <row r="18" spans="1:12" ht="20" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>32</v>
       </c>
@@ -1191,18 +1321,19 @@
       <c r="C18" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" s="2"/>
+      <c r="E18" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="F18" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="G18" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="J18" s="5"/>
-    </row>
-    <row r="19" spans="1:11" ht="20" x14ac:dyDescent="0.25">
+      <c r="K18" s="4"/>
+    </row>
+    <row r="19" spans="1:12" ht="20" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>35</v>
       </c>
@@ -1210,20 +1341,21 @@
       <c r="C19" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>117</v>
-      </c>
+      <c r="D19" s="2"/>
       <c r="E19" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="F19" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="G19" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I19" s="3"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="3"/>
-    </row>
-    <row r="20" spans="1:11" ht="20" x14ac:dyDescent="0.25">
+      <c r="J19" s="3"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="3"/>
+    </row>
+    <row r="20" spans="1:12" ht="20" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>35</v>
       </c>
@@ -1233,20 +1365,21 @@
       <c r="C20" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="D20" s="2" t="s">
-        <v>117</v>
-      </c>
+      <c r="D20" s="2"/>
       <c r="E20" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="F20" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="G20" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="I20" s="3"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="3"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J20" s="3"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="3"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>35</v>
       </c>
@@ -1255,14 +1388,15 @@
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
-      <c r="E21" s="2" t="s">
+      <c r="E21" s="2"/>
+      <c r="F21" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="G21" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="20" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" ht="20" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>37</v>
       </c>
@@ -1270,18 +1404,19 @@
       <c r="C22" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D22" s="2" t="s">
-        <v>117</v>
-      </c>
+      <c r="D22" s="2"/>
       <c r="E22" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="F22" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="G22" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J22" s="5"/>
-    </row>
-    <row r="23" spans="1:11" ht="20" x14ac:dyDescent="0.25">
+      <c r="K22" s="4"/>
+    </row>
+    <row r="23" spans="1:12" ht="20" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>37</v>
       </c>
@@ -1291,18 +1426,19 @@
       <c r="C23" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="D23" s="2" t="s">
-        <v>117</v>
-      </c>
+      <c r="D23" s="2"/>
       <c r="E23" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="F23" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="G23" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="J23" s="5"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K23" s="4"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>37</v>
       </c>
@@ -1311,14 +1447,15 @@
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
-      <c r="E24" s="2" t="s">
+      <c r="E24" s="2"/>
+      <c r="F24" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F24" s="2" t="s">
+      <c r="G24" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="20" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" ht="20" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>41</v>
       </c>
@@ -1326,20 +1463,21 @@
       <c r="C25" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="D25" s="2" t="s">
-        <v>117</v>
-      </c>
+      <c r="D25" s="2"/>
       <c r="E25" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="F25" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F25" s="2" t="s">
+      <c r="G25" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I25" s="3"/>
-      <c r="J25" s="5"/>
-      <c r="K25" s="3"/>
-    </row>
-    <row r="26" spans="1:11" ht="20" x14ac:dyDescent="0.25">
+      <c r="J25" s="3"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="3"/>
+    </row>
+    <row r="26" spans="1:12" ht="20" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>41</v>
       </c>
@@ -1349,100 +1487,110 @@
       <c r="C26" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="D26" s="2" t="s">
-        <v>117</v>
-      </c>
+      <c r="D26" s="2"/>
       <c r="E26" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="F26" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F26" s="2" t="s">
+      <c r="G26" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="I26" s="3"/>
-      <c r="J26" s="5"/>
-      <c r="K26" s="3"/>
-    </row>
-    <row r="27" spans="1:11" ht="20" x14ac:dyDescent="0.25">
+      <c r="J26" s="3"/>
+      <c r="K26" s="4"/>
+      <c r="L26" s="3"/>
+    </row>
+    <row r="27" spans="1:12" ht="20" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="C27" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="D27" s="2" t="s">
-        <v>117</v>
-      </c>
+      <c r="D27" s="5"/>
       <c r="E27" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="F27" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F27" s="2" t="s">
+      <c r="G27" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="J27" s="5"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K27" s="4"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>43</v>
       </c>
+      <c r="C28" s="2" t="s">
+        <v>127</v>
+      </c>
       <c r="D28" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E28" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="F28" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F28" s="2" t="s">
+      <c r="G28" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="20" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" ht="20" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C29" s="6" t="s">
+      <c r="C29" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="D29" s="2" t="s">
-        <v>117</v>
-      </c>
+      <c r="D29" s="5"/>
       <c r="E29" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="F29" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F29" s="2" t="s">
+      <c r="G29" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="J29" s="5"/>
-    </row>
-    <row r="30" spans="1:11" ht="20" x14ac:dyDescent="0.25">
+      <c r="K29" s="4"/>
+    </row>
+    <row r="30" spans="1:12" ht="20" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C30" s="6" t="s">
+      <c r="C30" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="D30" s="5"/>
+      <c r="E30" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="E30" s="2" t="s">
+      <c r="F30" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F30" s="2" t="s">
+      <c r="G30" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="J30" s="5"/>
-    </row>
-    <row r="31" spans="1:11" ht="20" x14ac:dyDescent="0.25">
+      <c r="K30" s="4"/>
+    </row>
+    <row r="31" spans="1:12" ht="20" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>47</v>
       </c>
@@ -1450,54 +1598,65 @@
       <c r="C31" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="D31" s="2" t="s">
-        <v>117</v>
-      </c>
+      <c r="D31" s="2"/>
       <c r="E31" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="F31" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F31" s="2" t="s">
+      <c r="G31" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J31" s="5"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K31" s="4"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C32" s="2"/>
+      <c r="C32" s="2" t="s">
+        <v>129</v>
+      </c>
       <c r="D32" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E32" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="E32" s="2" t="s">
+      <c r="F32" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F32" s="2" t="s">
+      <c r="G32" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C33" s="2"/>
+      <c r="C33" s="2" t="s">
+        <v>130</v>
+      </c>
       <c r="D33" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E33" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="E33" s="2" t="s">
+      <c r="F33" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F33" s="2" t="s">
+      <c r="G33" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="20" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" ht="20" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>51</v>
       </c>
@@ -1505,54 +1664,65 @@
       <c r="C34" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="D34" s="2" t="s">
-        <v>117</v>
-      </c>
+      <c r="D34" s="2"/>
       <c r="E34" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="F34" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F34" s="2" t="s">
+      <c r="G34" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J34" s="5"/>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K34" s="4"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>51</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C35" s="2"/>
+      <c r="C35" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="D35" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="E35" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="E35" s="2" t="s">
+      <c r="F35" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F35" s="2" t="s">
+      <c r="G35" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>51</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C36" s="2"/>
+      <c r="C36" s="2" t="s">
+        <v>134</v>
+      </c>
       <c r="D36" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="E36" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="E36" s="2" t="s">
+      <c r="F36" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="F36" s="2" t="s">
+      <c r="G36" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="20" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" ht="20" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>57</v>
       </c>
@@ -1560,36 +1730,42 @@
       <c r="C37" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="D37" s="2"/>
+      <c r="E37" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="E37" s="2" t="s">
+      <c r="F37" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F37" s="2" t="s">
+      <c r="G37" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J37" s="5"/>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K37" s="4"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>57</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C38" s="2"/>
+      <c r="C38" s="2" t="s">
+        <v>137</v>
+      </c>
       <c r="D38" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="E38" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="E38" s="2" t="s">
+      <c r="F38" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F38" s="2" t="s">
+      <c r="G38" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="20" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" ht="20" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>57</v>
       </c>
@@ -1599,18 +1775,19 @@
       <c r="C39" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="D39" s="2"/>
+      <c r="E39" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="E39" s="2" t="s">
+      <c r="F39" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="F39" s="2" t="s">
+      <c r="G39" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="J39" s="5"/>
-    </row>
-    <row r="40" spans="1:11" ht="20" x14ac:dyDescent="0.25">
+      <c r="K39" s="4"/>
+    </row>
+    <row r="40" spans="1:12" ht="20" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>60</v>
       </c>
@@ -1618,20 +1795,21 @@
       <c r="C40" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="D40" s="2" t="s">
-        <v>117</v>
-      </c>
+      <c r="D40" s="2"/>
       <c r="E40" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="F40" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F40" s="2" t="s">
+      <c r="G40" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I40" s="3"/>
-      <c r="J40" s="5"/>
-      <c r="K40" s="3"/>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J40" s="3"/>
+      <c r="K40" s="4"/>
+      <c r="L40" s="3"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>60</v>
       </c>
@@ -1640,14 +1818,15 @@
       </c>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
-      <c r="E41" s="2" t="s">
+      <c r="E41" s="2"/>
+      <c r="F41" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F41" s="2" t="s">
+      <c r="G41" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="20" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" ht="20" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>60</v>
       </c>
@@ -1657,20 +1836,21 @@
       <c r="C42" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D42" s="2" t="s">
+      <c r="D42" s="2"/>
+      <c r="E42" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="E42" s="2" t="s">
+      <c r="F42" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F42" s="2" t="s">
+      <c r="G42" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="I42" s="3"/>
-      <c r="J42" s="5"/>
-      <c r="K42" s="3"/>
-    </row>
-    <row r="43" spans="1:11" ht="20" x14ac:dyDescent="0.25">
+      <c r="J42" s="3"/>
+      <c r="K42" s="4"/>
+      <c r="L42" s="3"/>
+    </row>
+    <row r="43" spans="1:12" ht="20" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>63</v>
       </c>
@@ -1678,18 +1858,19 @@
       <c r="C43" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="D43" s="2" t="s">
-        <v>117</v>
-      </c>
+      <c r="D43" s="2"/>
       <c r="E43" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="F43" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="F43" s="2" t="s">
+      <c r="G43" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J43" s="5"/>
-    </row>
-    <row r="44" spans="1:11" ht="20" x14ac:dyDescent="0.25">
+      <c r="K43" s="4"/>
+    </row>
+    <row r="44" spans="1:12" ht="20" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>63</v>
       </c>
@@ -1699,18 +1880,19 @@
       <c r="C44" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="D44" s="2" t="s">
+      <c r="D44" s="2"/>
+      <c r="E44" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="E44" s="2" t="s">
+      <c r="F44" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F44" s="2" t="s">
+      <c r="G44" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="J44" s="5"/>
-    </row>
-    <row r="45" spans="1:11" ht="20" x14ac:dyDescent="0.25">
+      <c r="K44" s="4"/>
+    </row>
+    <row r="45" spans="1:12" ht="20" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>63</v>
       </c>
@@ -1720,18 +1902,19 @@
       <c r="C45" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="D45" s="2" t="s">
-        <v>117</v>
-      </c>
+      <c r="D45" s="2"/>
       <c r="E45" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="F45" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F45" s="2" t="s">
+      <c r="G45" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="J45" s="5"/>
-    </row>
-    <row r="46" spans="1:11" ht="20" x14ac:dyDescent="0.25">
+      <c r="K45" s="4"/>
+    </row>
+    <row r="46" spans="1:12" ht="20" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>67</v>
       </c>
@@ -1739,18 +1922,19 @@
       <c r="C46" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D46" s="2" t="s">
-        <v>117</v>
-      </c>
+      <c r="D46" s="2"/>
       <c r="E46" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="F46" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="F46" s="2" t="s">
+      <c r="G46" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J46" s="5"/>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K46" s="4"/>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>67</v>
       </c>
@@ -1759,14 +1943,15 @@
       </c>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
-      <c r="E47" s="2" t="s">
+      <c r="E47" s="2"/>
+      <c r="F47" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F47" s="2" t="s">
+      <c r="G47" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="48" spans="1:11" ht="20" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" ht="20" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>69</v>
       </c>
@@ -1774,18 +1959,19 @@
       <c r="C48" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="D48" s="2" t="s">
-        <v>117</v>
-      </c>
+      <c r="D48" s="2"/>
       <c r="E48" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="F48" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="F48" s="2" t="s">
+      <c r="G48" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J48" s="5"/>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K48" s="4"/>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>69</v>
       </c>
@@ -1794,14 +1980,15 @@
       </c>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
-      <c r="E49" s="2" t="s">
+      <c r="E49" s="2"/>
+      <c r="F49" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F49" s="2" t="s">
+      <c r="G49" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="50" spans="1:10" ht="20" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" ht="20" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>70</v>
       </c>
@@ -1809,144 +1996,180 @@
       <c r="C50" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="D50" s="2" t="s">
-        <v>117</v>
-      </c>
+      <c r="D50" s="2"/>
       <c r="E50" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="F50" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F50" s="2" t="s">
+      <c r="G50" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J50" s="5"/>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K50" s="4"/>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>70</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C51" s="2"/>
+      <c r="C51" s="2" t="s">
+        <v>139</v>
+      </c>
       <c r="D51" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="E51" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="E51" s="2" t="s">
+      <c r="F51" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F51" s="2" t="s">
+      <c r="G51" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>70</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C52" s="2"/>
+      <c r="C52" s="2" t="s">
+        <v>140</v>
+      </c>
       <c r="D52" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="E52" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="E52" s="2" t="s">
+      <c r="F52" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F52" s="2" t="s">
+      <c r="G52" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
         <v>70</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C53" s="2"/>
+      <c r="C53" s="2" t="s">
+        <v>141</v>
+      </c>
       <c r="D53" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E53" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="E53" s="2" t="s">
+      <c r="F53" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F53" s="2" t="s">
+      <c r="G53" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
         <v>70</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C54" s="2"/>
+      <c r="C54" s="2" t="s">
+        <v>142</v>
+      </c>
       <c r="D54" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="E54" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="E54" s="2" t="s">
+      <c r="F54" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F54" s="2" t="s">
+      <c r="G54" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>70</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C55" s="2"/>
+      <c r="C55" s="2" t="s">
+        <v>143</v>
+      </c>
       <c r="D55" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="E55" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="E55" s="2" t="s">
+      <c r="F55" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F55" s="2" t="s">
+      <c r="G55" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
         <v>70</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C56" s="2"/>
+      <c r="C56" s="2" t="s">
+        <v>144</v>
+      </c>
       <c r="D56" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="E56" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="E56" s="2" t="s">
+      <c r="F56" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F56" s="2" t="s">
+      <c r="G56" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>70</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C57" s="2"/>
+      <c r="C57" s="2" t="s">
+        <v>145</v>
+      </c>
       <c r="D57" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E57" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="E57" s="2" t="s">
+      <c r="F57" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F57" s="2" t="s">
+      <c r="G57" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="58" spans="1:10" ht="20" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" ht="20" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>78</v>
       </c>
@@ -1954,16 +2177,17 @@
       <c r="C58" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="D58" s="2" t="s">
-        <v>117</v>
-      </c>
+      <c r="D58" s="2"/>
       <c r="E58" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="F58" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F58" s="2" t="s">
+      <c r="G58" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J58" s="5"/>
+      <c r="K58" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>